<commit_message>
Made in tabular form
</commit_message>
<xml_diff>
--- a/Engineering/Requirements Development and Management/TMPL_CUSTFB.xlsx
+++ b/Engineering/Requirements Development and Management/TMPL_CUSTFB.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Revision History" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Customer Feedback Form</t>
   </si>
@@ -50,20 +50,26 @@
     <t>Decision Date</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t xml:space="preserve">Expected date If Approved </t>
   </si>
   <si>
     <t>Template Version 1</t>
+  </si>
+  <si>
+    <t>Remarks / Decision by Design</t>
+  </si>
+  <si>
+    <t>Received by</t>
+  </si>
+  <si>
+    <t>Expected Date (if approved)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +115,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -228,22 +250,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="4"/>
@@ -251,6 +263,38 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="40% - Accent1" xfId="3" builtinId="31"/>
@@ -259,9 +303,16 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="11">
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -272,12 +323,86 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
           <color indexed="64"/>
@@ -288,8 +413,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -326,11 +449,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A12:B24" totalsRowShown="0" tableBorderDxfId="3" totalsRowBorderDxfId="2" headerRowCellStyle="Heading 1">
-  <autoFilter ref="A12:B24"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Suggestions:" dataDxfId="1"/>
-    <tableColumn id="2" name="Descriptions" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A12:G24" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" tableBorderDxfId="10" totalsRowBorderDxfId="9" headerRowCellStyle="Heading 1">
+  <autoFilter ref="A12:G24"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Suggestions:" dataDxfId="8"/>
+    <tableColumn id="2" name="Descriptions" dataDxfId="7"/>
+    <tableColumn id="5" name="Received by" dataDxfId="6"/>
+    <tableColumn id="6" name="Received Date" dataDxfId="5"/>
+    <tableColumn id="3" name="Remarks / Decision by Design" dataDxfId="4"/>
+    <tableColumn id="4" name="Decision Date" dataDxfId="3"/>
+    <tableColumn id="7" name="Expected Date (if approved)" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -411,6 +539,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -445,6 +574,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -620,23 +750,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:1" ht="22.5">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:1" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" thickBot="1">
-      <c r="A4" s="13" t="s">
-        <v>13</v>
+    <row r="4" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -645,143 +775,234 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:F37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H37"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5703125" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="22.5">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:8" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-    </row>
-    <row r="4" spans="1:6" ht="19.5">
-      <c r="A4" s="14" t="s">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="14"/>
-    </row>
-    <row r="6" spans="1:6" ht="19.5">
-      <c r="A6" s="14" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="6" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="14"/>
-    </row>
-    <row r="8" spans="1:6" ht="19.5">
-      <c r="A8" s="14" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="8" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="14"/>
-    </row>
-    <row r="9" spans="1:6" ht="19.5">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-    </row>
-    <row r="10" spans="1:6" ht="19.5">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-    </row>
-    <row r="12" spans="1:6" ht="20.25" thickBot="1">
+      <c r="B8" s="8"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="12" spans="1:8" ht="59.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="20.25" customHeight="1" thickTop="1">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="E14" t="s">
+      <c r="C12" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="17"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="19" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3"/>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="2"/>
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="2"/>
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
-    </row>
-    <row r="27" spans="1:2" ht="15.75">
-      <c r="A27" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="15"/>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" ht="30.75" customHeight="1">
-      <c r="A37" s="11" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -793,7 +1014,7 @@
     <mergeCell ref="A27:B27"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B33:D33">
       <formula1>"Rejected, Approved,Need more info,Hold"</formula1>
     </dataValidation>
   </dataValidations>
@@ -806,21 +1027,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010005A068604E74C047BC66B3ED07869872" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7d65b694ac3f1c289d6201da35c196e2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -869,10 +1075,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E675935-B056-4A2C-844C-FFCF18C160F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B06B87C-695C-4272-833C-03EB6A468D29}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -892,16 +1120,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B06B87C-695C-4272-833C-03EB6A468D29}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E675935-B056-4A2C-844C-FFCF18C160F6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>